<commit_message>
update on product categories
</commit_message>
<xml_diff>
--- a/ExcelUtils/JB_Windows_TestMasterData.xlsx
+++ b/ExcelUtils/JB_Windows_TestMasterData.xlsx
@@ -170,21 +170,24 @@
     <t>Buy Two Get 30% Discount On Third</t>
   </si>
   <si>
+    <t>New Category1</t>
+  </si>
+  <si>
+    <t>E:\AutomationPhotos\Tomato.jpeg</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
+  <si>
+    <t>Buy One Get Two Free</t>
+  </si>
+  <si>
     <t>Foot Ware</t>
   </si>
   <si>
-    <t>E:\AutomationPhotos\Tomato.jpeg</t>
-  </si>
-  <si>
-    <t>Buy One Get Two Free</t>
-  </si>
-  <si>
     <t>Buy Two Get 50% Discount On Third</t>
   </si>
   <si>
-    <t>New Category1</t>
-  </si>
-  <si>
     <t>Eyeliner</t>
   </si>
   <si>
@@ -195,9 +198,6 @@
   </si>
   <si>
     <t>Complimentary</t>
-  </si>
-  <si>
-    <t>Vegetable</t>
   </si>
   <si>
     <t>Packing Charges</t>
@@ -6583,7 +6583,7 @@
   </sheetPr>
   <dimension ref="A1:M125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -6781,24 +6781,24 @@
         <v>36</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>24</v>
@@ -6809,7 +6809,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>14</v>
@@ -6827,13 +6827,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
@@ -6845,13 +6845,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
@@ -6863,7 +6863,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>14</v>
@@ -6889,7 +6889,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
@@ -6907,7 +6907,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
@@ -6925,7 +6925,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
@@ -6943,7 +6943,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
@@ -6961,7 +6961,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
@@ -6979,7 +6979,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
@@ -6997,7 +6997,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
@@ -7015,7 +7015,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13" t="s">
@@ -7033,7 +7033,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13" t="s">
@@ -7051,7 +7051,7 @@
         <v>14</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -11480,7 +11480,7 @@
         <v>163</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>164</v>
@@ -11525,7 +11525,7 @@
         <v>165</v>
       </c>
       <c r="V9" s="59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W9" s="59" t="s">
         <v>139</v>
@@ -11562,7 +11562,7 @@
         <v>168</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>148</v>
@@ -11620,7 +11620,7 @@
         <v>171</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>148</v>
@@ -12499,7 +12499,7 @@
         <v>209</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>148</v>
@@ -12544,7 +12544,7 @@
         <v>211</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>148</v>
@@ -12589,7 +12589,7 @@
         <v>213</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>148</v>
@@ -13399,7 +13399,7 @@
         <v>259</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>148</v>
@@ -13444,7 +13444,7 @@
         <v>262</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>148</v>
@@ -13489,7 +13489,7 @@
         <v>265</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>148</v>
@@ -14299,7 +14299,7 @@
         <v>319</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>148</v>
@@ -14344,7 +14344,7 @@
         <v>322</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F70" s="11" t="s">
         <v>148</v>
@@ -19063,7 +19063,7 @@
         <v>908</v>
       </c>
       <c r="E233" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F233" s="11" t="s">
         <v>148</v>
@@ -19084,7 +19084,7 @@
         <v>910</v>
       </c>
       <c r="E234" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F234" s="11" t="s">
         <v>148</v>
@@ -19105,7 +19105,7 @@
         <v>912</v>
       </c>
       <c r="E235" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F235" s="11" t="s">
         <v>148</v>
@@ -19126,7 +19126,7 @@
         <v>914</v>
       </c>
       <c r="E236" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F236" s="11" t="s">
         <v>148</v>
@@ -19147,7 +19147,7 @@
         <v>916</v>
       </c>
       <c r="E237" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F237" s="11" t="s">
         <v>148</v>
@@ -19168,7 +19168,7 @@
         <v>918</v>
       </c>
       <c r="E238" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F238" s="11" t="s">
         <v>148</v>
@@ -19189,7 +19189,7 @@
         <v>920</v>
       </c>
       <c r="E239" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F239" s="11" t="s">
         <v>148</v>
@@ -19210,7 +19210,7 @@
         <v>922</v>
       </c>
       <c r="E240" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F240" s="11" t="s">
         <v>148</v>
@@ -19231,7 +19231,7 @@
         <v>924</v>
       </c>
       <c r="E241" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F241" s="11" t="s">
         <v>148</v>
@@ -19252,7 +19252,7 @@
         <v>926</v>
       </c>
       <c r="E242" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F242" s="11" t="s">
         <v>148</v>
@@ -19273,7 +19273,7 @@
         <v>928</v>
       </c>
       <c r="E243" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F243" s="11" t="s">
         <v>148</v>
@@ -19294,7 +19294,7 @@
         <v>930</v>
       </c>
       <c r="E244" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F244" s="11" t="s">
         <v>148</v>
@@ -19315,7 +19315,7 @@
         <v>932</v>
       </c>
       <c r="E245" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F245" s="11" t="s">
         <v>148</v>
@@ -19336,7 +19336,7 @@
         <v>934</v>
       </c>
       <c r="E246" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F246" s="11" t="s">
         <v>148</v>
@@ -19357,7 +19357,7 @@
         <v>936</v>
       </c>
       <c r="E247" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F247" s="11" t="s">
         <v>148</v>
@@ -19378,7 +19378,7 @@
         <v>938</v>
       </c>
       <c r="E248" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F248" s="11" t="s">
         <v>148</v>
@@ -19399,7 +19399,7 @@
         <v>940</v>
       </c>
       <c r="E249" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F249" s="11" t="s">
         <v>148</v>
@@ -19420,7 +19420,7 @@
         <v>942</v>
       </c>
       <c r="E250" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F250" s="11" t="s">
         <v>148</v>
@@ -19441,7 +19441,7 @@
         <v>944</v>
       </c>
       <c r="E251" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F251" s="11" t="s">
         <v>148</v>
@@ -19462,7 +19462,7 @@
         <v>946</v>
       </c>
       <c r="E252" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F252" s="11" t="s">
         <v>148</v>

</xml_diff>